<commit_message>
Not sure what has been done here.
</commit_message>
<xml_diff>
--- a/replicape-display-BOM.xlsx
+++ b/replicape-display-BOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>WM7706TR-ND</t>
   </si>
@@ -46,6 +46,29 @@
   <si>
     <t>22uF Tantalum</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HFN404CT-ND</t>
+  </si>
+  <si>
+    <t>4 pin touch connector</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CONN FPC/FFC 4POS .5MM SMD GOLD</t>
+  </si>
+  <si>
+    <t>296-27010-1-ND</t>
+  </si>
+  <si>
+    <t>DC-DC conv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BSS138CT-ND</t>
+  </si>
+  <si>
+    <t>MOSFET N-CH 50V 220MA SOT-23</t>
   </si>
 </sst>
 </file>
@@ -419,15 +442,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -435,12 +462,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="14">
+    <row r="2" spans="1:3" ht="14">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="14">
+    <row r="3" spans="1:3" ht="14">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -448,17 +475,44 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="14">
+    <row r="4" spans="1:3" ht="14">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="14">
+    <row r="5" spans="1:3" ht="14">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="14">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="14">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="14">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>